<commit_message>
Improved sample spreadsheets for tests
</commit_message>
<xml_diff>
--- a/tests/sample_questionnaire.xlsx
+++ b/tests/sample_questionnaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcasalaina/src/QuestionnaireAgent_v2/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\QuestionnaireAgent_v2\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22677AA2-B7EC-5849-BB71-2DA6CBE74174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BAC645-B8BE-466D-98E7-317C2EEFE403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18195" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="4" r:id="rId1"/>
@@ -38,21 +38,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Please provide your company’s name</t>
   </si>
   <si>
     <t>Please specify the year your company was founded</t>
-  </si>
-  <si>
-    <t>How does your platform facilitate stakeholder alignment and documentation of ethical, legal, regulatory, and business considerations from project inception through AI project scoping and planning?</t>
-  </si>
-  <si>
-    <t>What capabilities does your platform provide for conducting algorithmic impact assessments to identify potential risks, biases, and societal implications prior to AI development?</t>
-  </si>
-  <si>
-    <t>How does your system enable the definition, tracking, and reporting of success criteria, fairness metrics, and governance KPIs throughout the entire AI project lifecycle?</t>
   </si>
   <si>
     <t>Q#</t>
@@ -101,6 +92,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Does your platform provide speech to text capabilities?</t>
+  </si>
+  <si>
+    <t>Does your platform provide text to speech capabilities?</t>
+  </si>
+  <si>
+    <t>How many languages does your text to speech capability support?</t>
+  </si>
+  <si>
+    <t>How many languages does your speech to text capability support?</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,6 +201,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3125,7 +3131,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1332F6B-6A1B-4855-AAD8-4326A0426458}" name="Table2" displayName="Table2" ref="A1:F4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1332F6B-6A1B-4855-AAD8-4326A0426458}" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DCA9A6B5-C9CF-48C8-9743-60B7AB3858D7}" name="Status" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{20231ED9-EF85-419F-B5C2-C512293F1CB8}" name="Owner" dataDxfId="12"/>
@@ -3403,43 +3409,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0833042D-20B2-4B8D-8BAE-92F7A65D9BAC}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="3" width="10.6640625" style="1" customWidth="1"/>
     <col min="4" max="6" width="60.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="5">
@@ -3451,23 +3457,23 @@
       <c r="E2" s="7"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5">
@@ -3516,103 +3522,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="3" width="10.6640625" style="3" customWidth="1"/>
     <col min="4" max="6" width="60.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="3"/>
+    <col min="7" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3">
-        <v>78</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3">
-        <v>79</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3">
-        <v>80</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:6" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:6" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="64" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="48" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:A4">
+  <conditionalFormatting sqref="A2:A5">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"final"</formula>
     </cfRule>
@@ -3638,7 +3632,7 @@
           <x14:formula1>
             <xm:f>Dashboard!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A4</xm:sqref>
+          <xm:sqref>A2:A5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3654,55 +3648,55 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" t="e">
         <f>COUNTIF(Table4[Status],Dashboard!A1)+COUNTIF(#REF!,Dashboard!A1)+COUNTIF(Table2[Status],Dashboard!A1)+COUNTIF(#REF!,Dashboard!A1)+COUNTIF(#REF!,Dashboard!A1)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" t="e">
         <f>COUNTIF(Table4[Status],Dashboard!A2)+COUNTIF(#REF!,Dashboard!A2)+COUNTIF(Table2[Status],Dashboard!A2)+COUNTIF(#REF!,Dashboard!A2)+COUNTIF(#REF!,Dashboard!A2)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="e">
         <f>COUNTIF(Table4[Status],Dashboard!A3)+COUNTIF(#REF!,Dashboard!A3)+COUNTIF(Table2[Status],Dashboard!A3)+COUNTIF(#REF!,Dashboard!A3)+COUNTIF(#REF!,Dashboard!A3)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="e">
         <f>COUNTIF(Table4[Status],Dashboard!A4)+COUNTIF(#REF!,Dashboard!A4)+COUNTIF(Table2[Status],Dashboard!A4)+COUNTIF(#REF!,Dashboard!A4)+COUNTIF(#REF!,Dashboard!A4)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" t="e">
         <f>COUNTBLANK(Table4[Documentation])+COUNTBLANK(#REF!)+COUNTBLANK(Table2[Documentation])+COUNTBLANK(#REF!)+COUNTBLANK(#REF!)</f>
@@ -3713,17 +3707,17 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" t="e">
         <f>COUNTBLANK(Table4[Owner])+COUNTBLANK(#REF!)+COUNTBLANK(Table2[Owner])+COUNTBLANK(#REF!)+COUNTBLANK(#REF!)</f>
@@ -3741,23 +3735,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5712b37e-f186-4b7d-ac1f-1d5cc166f78f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <SharedWithUsers xmlns="d087834a-fbb9-4346-a7f5-19fea6dcbccb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4050,29 +4033,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5712b37e-f186-4b7d-ac1f-1d5cc166f78f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <SharedWithUsers xmlns="d087834a-fbb9-4346-a7f5-19fea6dcbccb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955FCBAF-F542-47BE-B20A-2A8F8D83ACA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB2F6D5D-F98B-42E9-9D94-DB8B3598BFEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="d087834a-fbb9-4346-a7f5-19fea6dcbccb"/>
-    <ds:schemaRef ds:uri="5712b37e-f186-4b7d-ac1f-1d5cc166f78f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4099,9 +4082,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB2F6D5D-F98B-42E9-9D94-DB8B3598BFEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955FCBAF-F542-47BE-B20A-2A8F8D83ACA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="5712b37e-f186-4b7d-ac1f-1d5cc166f78f"/>
+    <ds:schemaRef ds:uri="d087834a-fbb9-4346-a7f5-19fea6dcbccb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>